<commit_message>
Proforma : formattage du code couleur sur 3 caractères
</commit_message>
<xml_diff>
--- a/Proforma/2018 12/extractionProformaFormatTxt.xlsx
+++ b/Proforma/2018 12/extractionProformaFormatTxt.xlsx
@@ -421,7 +421,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,6 +458,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -471,7 +477,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -481,6 +487,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2724,8 +2731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N20" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17:R35"/>
+    <sheetView tabSelected="1" topLeftCell="K17" workbookViewId="0">
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3282,8 +3289,8 @@
         <f t="shared" ca="1" si="11"/>
         <v>ECS07</v>
       </c>
-      <c r="M20" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="M20" s="7" t="str">
+        <f t="shared" ref="M20:M57" ca="1" si="12">RIGHT("000" &amp; TRIM(INDEX(INDIRECT($G20),OFFSET(INDIRECT($E20), 0, COLUMN(M20)-1)+$B20-1)), 3)</f>
         <v>133</v>
       </c>
       <c r="N20" t="str">
@@ -3325,7 +3332,7 @@
         <v>7</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" ref="E21:E57" ca="1" si="12">"A" &amp; D21</f>
+        <f t="shared" ref="E21:E57" ca="1" si="13">"A" &amp; D21</f>
         <v>A7</v>
       </c>
       <c r="F21">
@@ -3337,7 +3344,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J21" t="str">
-        <f t="shared" ref="J21:R36" ca="1" si="13">TRIM(INDEX(INDIRECT($G21),OFFSET(INDIRECT($E21), 0, COLUMN(J21)-1)+$B21-1))</f>
+        <f t="shared" ref="J21:R36" ca="1" si="14">TRIM(INDEX(INDIRECT($G21),OFFSET(INDIRECT($E21), 0, COLUMN(J21)-1)+$B21-1))</f>
         <v>16</v>
       </c>
       <c r="K21" t="str">
@@ -3348,8 +3355,8 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M21" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="M21" s="7" t="str">
+        <f t="shared" ca="1" si="12"/>
         <v>389</v>
       </c>
       <c r="N21" t="str">
@@ -3357,15 +3364,15 @@
         <v>UNICA</v>
       </c>
       <c r="O21" s="6">
-        <f t="shared" ref="O21:Q57" ca="1" si="14">0+TRIM(INDEX(INDIRECT($G21),OFFSET(INDIRECT($E21), 0, COLUMN(O21)-1)+$B21-1))</f>
+        <f t="shared" ref="O21:Q57" ca="1" si="15">0+TRIM(INDEX(INDIRECT($G21),OFFSET(INDIRECT($E21), 0, COLUMN(O21)-1)+$B21-1))</f>
         <v>8</v>
       </c>
       <c r="P21" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14.4</v>
       </c>
       <c r="Q21" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>115.2</v>
       </c>
       <c r="R21" t="str">
@@ -3375,11 +3382,11 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f t="shared" ref="A22:A34" ca="1" si="15">IF(B21=C21,A21+1,A21)</f>
+        <f t="shared" ref="A22:A34" ca="1" si="16">IF(B21=C21,A21+1,A21)</f>
         <v>1</v>
       </c>
       <c r="B22">
-        <f t="shared" ref="B22:B33" ca="1" si="16">IF(A22=A21,B21+1,1)</f>
+        <f t="shared" ref="B22:B33" ca="1" si="17">IF(A22=A21,B21+1,1)</f>
         <v>3</v>
       </c>
       <c r="C22">
@@ -3391,7 +3398,7 @@
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F22">
@@ -3403,7 +3410,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J22" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>3</v>
       </c>
       <c r="K22" t="str">
@@ -3414,8 +3421,8 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M22" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="M22" s="7" t="str">
+        <f t="shared" ca="1" si="12"/>
         <v>389</v>
       </c>
       <c r="N22" t="str">
@@ -3423,15 +3430,15 @@
         <v>UNICA</v>
       </c>
       <c r="O22" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10</v>
       </c>
       <c r="P22" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14.4</v>
       </c>
       <c r="Q22" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>144</v>
       </c>
       <c r="R22" t="str">
@@ -3441,11 +3448,11 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B23">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>4</v>
       </c>
       <c r="C23">
@@ -3457,7 +3464,7 @@
         <v>7</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F23">
@@ -3469,7 +3476,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J23" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>9</v>
       </c>
       <c r="K23" t="str">
@@ -3480,24 +3487,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M23" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>17</v>
+      <c r="M23" s="7" t="str">
+        <f ca="1">RIGHT("000" &amp; TRIM(INDEX(INDIRECT($G23),OFFSET(INDIRECT($E23), 0, COLUMN(M23)-1)+$B23-1)), 3)</f>
+        <v>017</v>
       </c>
       <c r="N23" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O23" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3</v>
       </c>
       <c r="P23" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14.16</v>
       </c>
       <c r="Q23" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>42.48</v>
       </c>
       <c r="R23" t="str">
@@ -3507,11 +3514,11 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B24">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>5</v>
       </c>
       <c r="C24">
@@ -3523,7 +3530,7 @@
         <v>7</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F24">
@@ -3535,35 +3542,35 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J24" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>8</v>
-      </c>
-      <c r="K24" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>OBAGB001</v>
-      </c>
-      <c r="L24" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>EVS00</v>
-      </c>
-      <c r="M24" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>24</v>
-      </c>
-      <c r="N24" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>UNICA</v>
-      </c>
-      <c r="O24" s="6">
         <f t="shared" ca="1" si="14"/>
         <v>8</v>
       </c>
+      <c r="K24" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>OBAGB001</v>
+      </c>
+      <c r="L24" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>EVS00</v>
+      </c>
+      <c r="M24" s="7" t="str">
+        <f t="shared" ref="M24:M57" ca="1" si="18">RIGHT("000" &amp; TRIM(INDEX(INDIRECT($G24),OFFSET(INDIRECT($E24), 0, COLUMN(M24)-1)+$B24-1)), 3)</f>
+        <v>024</v>
+      </c>
+      <c r="N24" t="str">
+        <f t="shared" ca="1" si="11"/>
+        <v>UNICA</v>
+      </c>
+      <c r="O24" s="6">
+        <f t="shared" ca="1" si="15"/>
+        <v>8</v>
+      </c>
       <c r="P24" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14.4</v>
       </c>
       <c r="Q24" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>115.2</v>
       </c>
       <c r="R24" t="str">
@@ -3573,11 +3580,11 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B25">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>6</v>
       </c>
       <c r="C25">
@@ -3589,7 +3596,7 @@
         <v>7</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F25">
@@ -3601,7 +3608,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J25" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>5</v>
       </c>
       <c r="K25" t="str">
@@ -3612,8 +3619,8 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M25" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="M25" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
         <v>541</v>
       </c>
       <c r="N25" t="str">
@@ -3621,15 +3628,15 @@
         <v>UNICA</v>
       </c>
       <c r="O25" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>6</v>
       </c>
       <c r="P25" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14.4</v>
       </c>
       <c r="Q25" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>86.4</v>
       </c>
       <c r="R25" t="str">
@@ -3639,11 +3646,11 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B26">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>7</v>
       </c>
       <c r="C26">
@@ -3655,7 +3662,7 @@
         <v>7</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F26">
@@ -3667,7 +3674,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J26" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>2</v>
       </c>
       <c r="K26" t="str">
@@ -3678,24 +3685,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M26" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>78</v>
+      <c r="M26" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>078</v>
       </c>
       <c r="N26" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O26" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3</v>
       </c>
       <c r="P26" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>14.16</v>
       </c>
       <c r="Q26" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>42.48</v>
       </c>
       <c r="R26" t="str">
@@ -3705,11 +3712,11 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B27">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>8</v>
       </c>
       <c r="C27">
@@ -3721,7 +3728,7 @@
         <v>7</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F27">
@@ -3733,7 +3740,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J27" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>13</v>
       </c>
       <c r="K27" t="str">
@@ -3744,24 +3751,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M27" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>24</v>
+      <c r="M27" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>024</v>
       </c>
       <c r="N27" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O27" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>2</v>
       </c>
       <c r="P27" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>11.88</v>
       </c>
       <c r="Q27" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>23.76</v>
       </c>
       <c r="R27" t="str">
@@ -3771,11 +3778,11 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B28">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>9</v>
       </c>
       <c r="C28">
@@ -3787,7 +3794,7 @@
         <v>7</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F28">
@@ -3799,7 +3806,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J28" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>6</v>
       </c>
       <c r="K28" t="str">
@@ -3810,24 +3817,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M28" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>71</v>
+      <c r="M28" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>071</v>
       </c>
       <c r="N28" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O28" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>2</v>
       </c>
       <c r="P28" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>11.88</v>
       </c>
       <c r="Q28" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>23.76</v>
       </c>
       <c r="R28" t="str">
@@ -3837,11 +3844,11 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B29">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>10</v>
       </c>
       <c r="C29">
@@ -3853,7 +3860,7 @@
         <v>7</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F29">
@@ -3865,7 +3872,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J29" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>4</v>
       </c>
       <c r="K29" t="str">
@@ -3876,24 +3883,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>EVS00</v>
       </c>
-      <c r="M29" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>24</v>
+      <c r="M29" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>024</v>
       </c>
       <c r="N29" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O29" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>5</v>
       </c>
       <c r="P29" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>4.8</v>
       </c>
       <c r="Q29" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>24</v>
       </c>
       <c r="R29" t="str">
@@ -3903,11 +3910,11 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B30">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>11</v>
       </c>
       <c r="C30">
@@ -3919,7 +3926,7 @@
         <v>7</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F30">
@@ -3931,7 +3938,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J30" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>14</v>
       </c>
       <c r="K30" t="str">
@@ -3942,24 +3949,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>TESR1</v>
       </c>
-      <c r="M30" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>18</v>
+      <c r="M30" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>018</v>
       </c>
       <c r="N30" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O30" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>5</v>
       </c>
       <c r="P30" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10.8</v>
       </c>
       <c r="Q30" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>54</v>
       </c>
       <c r="R30" t="str">
@@ -3969,11 +3976,11 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B31">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>12</v>
       </c>
       <c r="C31">
@@ -3985,7 +3992,7 @@
         <v>7</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F31">
@@ -3997,7 +4004,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J31" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>15</v>
       </c>
       <c r="K31" t="str">
@@ -4008,8 +4015,8 @@
         <f t="shared" ca="1" si="11"/>
         <v>TESR1</v>
       </c>
-      <c r="M31" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="M31" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
         <v>258</v>
       </c>
       <c r="N31" t="str">
@@ -4017,15 +4024,15 @@
         <v>UNICA</v>
       </c>
       <c r="O31" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>8</v>
       </c>
       <c r="P31" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>10.8</v>
       </c>
       <c r="Q31" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>86.4</v>
       </c>
       <c r="R31" t="str">
@@ -4035,11 +4042,11 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>1</v>
       </c>
       <c r="B32">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>13</v>
       </c>
       <c r="C32">
@@ -4051,7 +4058,7 @@
         <v>7</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A7</v>
       </c>
       <c r="F32">
@@ -4063,7 +4070,7 @@
         <v>'Données'!A1:A5001</v>
       </c>
       <c r="J32" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>10</v>
       </c>
       <c r="K32" t="str">
@@ -4074,24 +4081,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>TESR1</v>
       </c>
-      <c r="M32" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>18</v>
+      <c r="M32" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>018</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O32" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3</v>
       </c>
       <c r="P32" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>9</v>
       </c>
       <c r="Q32" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>27</v>
       </c>
       <c r="R32" t="str">
@@ -4101,11 +4108,11 @@
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>2</v>
       </c>
       <c r="B33">
-        <f t="shared" ca="1" si="16"/>
+        <f t="shared" ca="1" si="17"/>
         <v>1</v>
       </c>
       <c r="C33">
@@ -4117,7 +4124,7 @@
         <v>9</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A9</v>
       </c>
       <c r="F33">
@@ -4129,7 +4136,7 @@
         <v>'Données'!A210:A5210</v>
       </c>
       <c r="J33" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>12</v>
       </c>
       <c r="K33" t="str">
@@ -4140,24 +4147,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>TESR1</v>
       </c>
-      <c r="M33" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>86</v>
+      <c r="M33" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>086</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O33" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>5</v>
       </c>
       <c r="P33" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>9</v>
       </c>
       <c r="Q33" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>45</v>
       </c>
       <c r="R33" t="str">
@@ -4167,7 +4174,7 @@
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f t="shared" ca="1" si="15"/>
+        <f t="shared" ca="1" si="16"/>
         <v>2</v>
       </c>
       <c r="B34">
@@ -4183,7 +4190,7 @@
         <v>9</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A9</v>
       </c>
       <c r="F34">
@@ -4195,7 +4202,7 @@
         <v>'Données'!A210:A5210</v>
       </c>
       <c r="J34" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>11</v>
       </c>
       <c r="K34" t="str">
@@ -4206,8 +4213,8 @@
         <f t="shared" ca="1" si="11"/>
         <v>TESR1</v>
       </c>
-      <c r="M34" t="str">
-        <f t="shared" ca="1" si="11"/>
+      <c r="M34" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
         <v>258</v>
       </c>
       <c r="N34" t="str">
@@ -4215,15 +4222,15 @@
         <v>UNICA</v>
       </c>
       <c r="O34" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>3</v>
       </c>
       <c r="P34" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>9</v>
       </c>
       <c r="Q34" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>27</v>
       </c>
       <c r="R34" t="str">
@@ -4233,11 +4240,11 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f t="shared" ref="A35:A55" ca="1" si="17">IF(B34=C34,A34+1,A34)</f>
+        <f t="shared" ref="A35:A55" ca="1" si="19">IF(B34=C34,A34+1,A34)</f>
         <v>2</v>
       </c>
       <c r="B35">
-        <f t="shared" ref="B35:B41" ca="1" si="18">IF(A35=A34,B34+1,1)</f>
+        <f t="shared" ref="B35:B41" ca="1" si="20">IF(A35=A34,B34+1,1)</f>
         <v>3</v>
       </c>
       <c r="C35">
@@ -4249,7 +4256,7 @@
         <v>9</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A9</v>
       </c>
       <c r="F35">
@@ -4261,7 +4268,7 @@
         <v>'Données'!A210:A5210</v>
       </c>
       <c r="J35" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>7</v>
       </c>
       <c r="K35" t="str">
@@ -4272,24 +4279,24 @@
         <f t="shared" ca="1" si="11"/>
         <v>ECS00</v>
       </c>
-      <c r="M35" t="str">
-        <f t="shared" ca="1" si="11"/>
-        <v>18</v>
+      <c r="M35" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>018</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" ca="1" si="11"/>
         <v>UNICA</v>
       </c>
       <c r="O35" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>2</v>
       </c>
       <c r="P35" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>18.96</v>
       </c>
       <c r="Q35" s="6">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>37.92</v>
       </c>
       <c r="R35" t="str">
@@ -4299,11 +4306,11 @@
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>2</v>
       </c>
       <c r="B36">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>4</v>
       </c>
       <c r="C36">
@@ -4315,7 +4322,7 @@
         <v>9</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A9</v>
       </c>
       <c r="F36">
@@ -4327,49 +4334,49 @@
         <v>'Données'!A210:A5210</v>
       </c>
       <c r="J36" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>17</v>
       </c>
       <c r="K36" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>TESR1</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>000_SPTRASP</v>
       </c>
-      <c r="M36" t="str">
-        <f t="shared" ca="1" si="13"/>
-        <v>002489 O BAG STORE TOULOUSE</v>
+      <c r="M36" s="7" t="str">
+        <f t="shared" ca="1" si="18"/>
+        <v>USE</v>
       </c>
       <c r="N36" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" ca="1" si="14"/>
         <v>Taille</v>
       </c>
       <c r="O36" s="6">
+        <f t="shared" ca="1" si="15"/>
+        <v>9</v>
+      </c>
+      <c r="P36" s="6">
+        <f t="shared" ca="1" si="15"/>
+        <v>45</v>
+      </c>
+      <c r="Q36" s="6" t="e">
+        <f t="shared" ca="1" si="15"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="R36" t="str">
         <f t="shared" ca="1" si="14"/>
-        <v>9</v>
-      </c>
-      <c r="P36" s="6">
-        <f t="shared" ca="1" si="14"/>
-        <v>45</v>
-      </c>
-      <c r="Q36" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="R36" t="str">
-        <f t="shared" ca="1" si="13"/>
         <v>DÉBIT FRAIS DE TRANSPORT</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>3</v>
       </c>
       <c r="B37">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>1</v>
       </c>
       <c r="C37" t="e">
@@ -4381,7 +4388,7 @@
         <v>11</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>A11</v>
       </c>
       <c r="F37">
@@ -4393,49 +4400,49 @@
         <v>'Données'!A363:A5363</v>
       </c>
       <c r="J37" t="e">
-        <f t="shared" ref="J37:R52" ca="1" si="19">TRIM(INDEX(INDIRECT($G37),OFFSET(INDIRECT($E37), 0, COLUMN(J37)-1)+$B37-1))</f>
+        <f t="shared" ref="J37:R52" ca="1" si="21">TRIM(INDEX(INDIRECT($G37),OFFSET(INDIRECT($E37), 0, COLUMN(J37)-1)+$B37-1))</f>
         <v>#N/A</v>
       </c>
       <c r="K37" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L37" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M37" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M37" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N37" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O37" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P37" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q37" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R37" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B38" t="e">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>#N/A</v>
       </c>
       <c r="C38" t="e">
@@ -4447,7 +4454,7 @@
         <v>#N/A</v>
       </c>
       <c r="E38" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F38" t="e">
@@ -4459,49 +4466,49 @@
         <v>#N/A</v>
       </c>
       <c r="J38" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K38" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L38" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M38" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M38" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N38" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O38" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P38" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q38" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R38" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B39" t="e">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>#N/A</v>
       </c>
       <c r="C39" t="e">
@@ -4513,7 +4520,7 @@
         <v>#N/A</v>
       </c>
       <c r="E39" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F39" t="e">
@@ -4525,49 +4532,49 @@
         <v>#N/A</v>
       </c>
       <c r="J39" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K39" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L39" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M39" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M39" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N39" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O39" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P39" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q39" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R39" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B40" t="e">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>#N/A</v>
       </c>
       <c r="C40" t="e">
@@ -4579,7 +4586,7 @@
         <v>#N/A</v>
       </c>
       <c r="E40" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F40" t="e">
@@ -4591,49 +4598,49 @@
         <v>#N/A</v>
       </c>
       <c r="J40" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K40" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L40" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M40" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M40" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N40" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O40" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P40" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q40" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R40" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B41" t="e">
-        <f t="shared" ca="1" si="18"/>
+        <f t="shared" ca="1" si="20"/>
         <v>#N/A</v>
       </c>
       <c r="C41" t="e">
@@ -4645,7 +4652,7 @@
         <v>#N/A</v>
       </c>
       <c r="E41" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F41" t="e">
@@ -4657,45 +4664,45 @@
         <v>#N/A</v>
       </c>
       <c r="J41" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K41" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L41" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M41" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M41" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N41" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O41" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P41" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q41" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R41" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B42" t="e">
@@ -4711,7 +4718,7 @@
         <v>#N/A</v>
       </c>
       <c r="E42" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F42" t="e">
@@ -4723,49 +4730,49 @@
         <v>#N/A</v>
       </c>
       <c r="J42" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K42" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L42" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M42" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M42" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N42" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O42" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P42" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q42" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R42" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B43" t="e">
-        <f t="shared" ref="B43:B45" ca="1" si="20">IF(A43=A42,B42+1,1)</f>
+        <f t="shared" ref="B43:B45" ca="1" si="22">IF(A43=A42,B42+1,1)</f>
         <v>#N/A</v>
       </c>
       <c r="C43" t="e">
@@ -4777,7 +4784,7 @@
         <v>#N/A</v>
       </c>
       <c r="E43" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F43" t="e">
@@ -4789,49 +4796,49 @@
         <v>#N/A</v>
       </c>
       <c r="J43" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K43" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L43" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M43" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M43" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N43" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O43" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P43" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q43" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R43" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B44" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#N/A</v>
       </c>
       <c r="C44" t="e">
@@ -4843,7 +4850,7 @@
         <v>#N/A</v>
       </c>
       <c r="E44" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F44" t="e">
@@ -4855,49 +4862,49 @@
         <v>#N/A</v>
       </c>
       <c r="J44" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K44" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L44" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M44" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M44" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N44" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O44" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P44" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q44" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R44" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B45" t="e">
-        <f t="shared" ca="1" si="20"/>
+        <f t="shared" ca="1" si="22"/>
         <v>#N/A</v>
       </c>
       <c r="C45" t="e">
@@ -4909,7 +4916,7 @@
         <v>#N/A</v>
       </c>
       <c r="E45" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F45" t="e">
@@ -4921,45 +4928,45 @@
         <v>#N/A</v>
       </c>
       <c r="J45" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K45" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L45" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M45" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M45" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N45" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O45" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P45" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q45" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R45" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B46" t="e">
@@ -4975,7 +4982,7 @@
         <v>#N/A</v>
       </c>
       <c r="E46" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F46" t="e">
@@ -4987,49 +4994,49 @@
         <v>#N/A</v>
       </c>
       <c r="J46" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K46" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L46" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M46" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M46" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N46" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O46" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P46" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q46" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R46" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B47" t="e">
-        <f t="shared" ref="B47" ca="1" si="21">IF(A47=A46,B46+1,1)</f>
+        <f t="shared" ref="B47" ca="1" si="23">IF(A47=A46,B46+1,1)</f>
         <v>#N/A</v>
       </c>
       <c r="C47" t="e">
@@ -5041,7 +5048,7 @@
         <v>#N/A</v>
       </c>
       <c r="E47" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F47" t="e">
@@ -5053,49 +5060,49 @@
         <v>#N/A</v>
       </c>
       <c r="J47" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K47" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L47" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M47" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M47" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N47" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O47" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P47" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q47" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R47" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B48" t="e">
-        <f t="shared" ref="B48:B50" ca="1" si="22">IF(A48=A47,B47+1,1)</f>
+        <f t="shared" ref="B48:B50" ca="1" si="24">IF(A48=A47,B47+1,1)</f>
         <v>#N/A</v>
       </c>
       <c r="C48" t="e">
@@ -5107,7 +5114,7 @@
         <v>#N/A</v>
       </c>
       <c r="E48" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F48" t="e">
@@ -5119,49 +5126,49 @@
         <v>#N/A</v>
       </c>
       <c r="J48" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K48" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L48" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M48" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M48" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N48" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O48" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P48" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q48" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R48" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B49" t="e">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#N/A</v>
       </c>
       <c r="C49" t="e">
@@ -5173,7 +5180,7 @@
         <v>#N/A</v>
       </c>
       <c r="E49" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F49" t="e">
@@ -5185,49 +5192,49 @@
         <v>#N/A</v>
       </c>
       <c r="J49" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K49" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L49" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M49" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M49" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N49" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O49" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P49" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q49" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R49" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" t="e">
-        <f t="shared" ref="A50" ca="1" si="23">IF(B49=C49,A49+1,A49)</f>
+        <f t="shared" ref="A50" ca="1" si="25">IF(B49=C49,A49+1,A49)</f>
         <v>#N/A</v>
       </c>
       <c r="B50" t="e">
-        <f t="shared" ca="1" si="22"/>
+        <f t="shared" ca="1" si="24"/>
         <v>#N/A</v>
       </c>
       <c r="C50" t="e">
@@ -5239,7 +5246,7 @@
         <v>#N/A</v>
       </c>
       <c r="E50" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F50" t="e">
@@ -5251,49 +5258,49 @@
         <v>#N/A</v>
       </c>
       <c r="J50" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K50" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L50" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M50" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M50" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N50" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O50" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P50" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q50" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R50" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B51" t="e">
-        <f t="shared" ref="B51:B55" ca="1" si="24">IF(A51=A50,B50+1,1)</f>
+        <f t="shared" ref="B51:B55" ca="1" si="26">IF(A51=A50,B50+1,1)</f>
         <v>#N/A</v>
       </c>
       <c r="C51" t="e">
@@ -5305,7 +5312,7 @@
         <v>#N/A</v>
       </c>
       <c r="E51" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F51" t="e">
@@ -5317,49 +5324,49 @@
         <v>#N/A</v>
       </c>
       <c r="J51" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K51" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L51" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M51" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M51" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N51" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O51" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P51" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q51" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R51" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B52" t="e">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="26"/>
         <v>#N/A</v>
       </c>
       <c r="C52" t="e">
@@ -5371,7 +5378,7 @@
         <v>#N/A</v>
       </c>
       <c r="E52" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F52" t="e">
@@ -5383,49 +5390,49 @@
         <v>#N/A</v>
       </c>
       <c r="J52" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="K52" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="L52" t="e">
-        <f t="shared" ca="1" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M52" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M52" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N52" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
       <c r="O52" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P52" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q52" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R52" t="e">
-        <f t="shared" ca="1" si="19"/>
+        <f t="shared" ca="1" si="21"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B53" t="e">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="26"/>
         <v>#N/A</v>
       </c>
       <c r="C53" t="e">
@@ -5437,7 +5444,7 @@
         <v>#N/A</v>
       </c>
       <c r="E53" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F53" t="e">
@@ -5449,49 +5456,49 @@
         <v>#N/A</v>
       </c>
       <c r="J53" t="e">
-        <f t="shared" ref="J53:R57" ca="1" si="25">TRIM(INDEX(INDIRECT($G53),OFFSET(INDIRECT($E53), 0, COLUMN(J53)-1)+$B53-1))</f>
+        <f t="shared" ref="J53:R57" ca="1" si="27">TRIM(INDEX(INDIRECT($G53),OFFSET(INDIRECT($E53), 0, COLUMN(J53)-1)+$B53-1))</f>
         <v>#N/A</v>
       </c>
       <c r="K53" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="L53" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M53" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M53" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N53" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="O53" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P53" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q53" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R53" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B54" t="e">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="26"/>
         <v>#N/A</v>
       </c>
       <c r="C54" t="e">
@@ -5503,7 +5510,7 @@
         <v>#N/A</v>
       </c>
       <c r="E54" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F54" t="e">
@@ -5515,49 +5522,49 @@
         <v>#N/A</v>
       </c>
       <c r="J54" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="K54" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="L54" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M54" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M54" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N54" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="O54" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P54" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q54" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R54" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" t="e">
-        <f t="shared" ca="1" si="17"/>
+        <f t="shared" ca="1" si="19"/>
         <v>#N/A</v>
       </c>
       <c r="B55" t="e">
-        <f t="shared" ca="1" si="24"/>
+        <f t="shared" ca="1" si="26"/>
         <v>#N/A</v>
       </c>
       <c r="C55" t="e">
@@ -5569,7 +5576,7 @@
         <v>#N/A</v>
       </c>
       <c r="E55" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F55" t="e">
@@ -5581,49 +5588,49 @@
         <v>#N/A</v>
       </c>
       <c r="J55" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="K55" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="L55" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M55" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M55" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N55" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="O55" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P55" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q55" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R55" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" t="e">
-        <f t="shared" ref="A56:A57" ca="1" si="26">IF(B55=C55,A55+1,A55)</f>
+        <f t="shared" ref="A56:A57" ca="1" si="28">IF(B55=C55,A55+1,A55)</f>
         <v>#N/A</v>
       </c>
       <c r="B56" t="e">
-        <f t="shared" ref="B56:B57" ca="1" si="27">IF(A56=A55,B55+1,1)</f>
+        <f t="shared" ref="B56:B57" ca="1" si="29">IF(A56=A55,B55+1,1)</f>
         <v>#N/A</v>
       </c>
       <c r="C56" t="e">
@@ -5635,7 +5642,7 @@
         <v>#N/A</v>
       </c>
       <c r="E56" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F56" t="e">
@@ -5647,49 +5654,49 @@
         <v>#N/A</v>
       </c>
       <c r="J56" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="K56" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="L56" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M56" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M56" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N56" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="O56" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P56" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q56" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R56" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" t="e">
-        <f t="shared" ca="1" si="26"/>
+        <f t="shared" ca="1" si="28"/>
         <v>#N/A</v>
       </c>
       <c r="B57" t="e">
-        <f t="shared" ca="1" si="27"/>
+        <f t="shared" ca="1" si="29"/>
         <v>#N/A</v>
       </c>
       <c r="C57" t="e">
@@ -5701,7 +5708,7 @@
         <v>#N/A</v>
       </c>
       <c r="E57" t="e">
-        <f t="shared" ca="1" si="12"/>
+        <f t="shared" ca="1" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="F57" t="e">
@@ -5713,39 +5720,39 @@
         <v>#N/A</v>
       </c>
       <c r="J57" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="K57" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="L57" t="e">
-        <f t="shared" ca="1" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="M57" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
+        <v>#N/A</v>
+      </c>
+      <c r="M57" s="7" t="e">
+        <f t="shared" ca="1" si="18"/>
         <v>#N/A</v>
       </c>
       <c r="N57" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
       <c r="O57" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="P57" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="Q57" s="6" t="e">
-        <f t="shared" ca="1" si="14"/>
+        <f t="shared" ca="1" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="R57" t="e">
-        <f t="shared" ca="1" si="25"/>
+        <f t="shared" ca="1" si="27"/>
         <v>#N/A</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Proforma : analyse OK des proformas
</commit_message>
<xml_diff>
--- a/Proforma/2018 12/extractionProformaFormatTxt.xlsx
+++ b/Proforma/2018 12/extractionProformaFormatTxt.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Données" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
   <definedNames>
     <definedName name="nomOngletDonnées">Feuil2!$C$2</definedName>
     <definedName name="referenceFacture">Feuil2!$J$4</definedName>
-    <definedName name="tabCodes">Feuil3!$A:$A</definedName>
+    <definedName name="tabCodes">Feuil3!$C:$C</definedName>
     <definedName name="totalFacture">Feuil2!$J$2</definedName>
     <definedName name="totalMontant">Feuil2!$J$3</definedName>
   </definedNames>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="140">
   <si>
     <t xml:space="preserve">SOFEA </t>
   </si>
@@ -398,6 +398,51 @@
   </si>
   <si>
     <t>Reference</t>
+  </si>
+  <si>
+    <t>LI</t>
+  </si>
+  <si>
+    <t>MO</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>UN</t>
+  </si>
+  <si>
+    <t>PI</t>
+  </si>
+  <si>
+    <t>QT</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>MT</t>
+  </si>
+  <si>
+    <t>TF</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>RF</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -2731,7 +2776,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K17" workbookViewId="0">
+    <sheetView topLeftCell="K17" workbookViewId="0">
       <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
@@ -3290,7 +3335,7 @@
         <v>ECS07</v>
       </c>
       <c r="M20" s="7" t="str">
-        <f t="shared" ref="M20:M57" ca="1" si="12">RIGHT("000" &amp; TRIM(INDEX(INDIRECT($G20),OFFSET(INDIRECT($E20), 0, COLUMN(M20)-1)+$B20-1)), 3)</f>
+        <f t="shared" ref="M20:M22" ca="1" si="12">RIGHT("000" &amp; TRIM(INDEX(INDIRECT($G20),OFFSET(INDIRECT($E20), 0, COLUMN(M20)-1)+$B20-1)), 3)</f>
         <v>133</v>
       </c>
       <c r="N20" t="str">
@@ -5772,76 +5817,154 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>129</v>
+      </c>
+      <c r="C7" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C8" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C9" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>137</v>
+      </c>
+      <c r="B12" t="s">
+        <v>134</v>
+      </c>
+      <c r="C12" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" t="s">
+        <v>135</v>
+      </c>
+      <c r="C13" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>